<commit_message>
Fixed run_rothc_grassland_scenarios... and loading of excel file of scenarios
</commit_message>
<xml_diff>
--- a/data/grasslands/grassland_baseline_rothc_scenarios.xlsx
+++ b/data/grasslands/grassland_baseline_rothc_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/grasslands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{A4062F05-E793-4E32-8DC1-6F3E9D7BC553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14BAD5AD-4A27-461A-B54A-2629284719D3}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{A4062F05-E793-4E32-8DC1-6F3E9D7BC553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34442E2E-2248-469D-B323-A592B8C21F85}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{67808942-AFB5-48B3-8BA1-0FBB84EB6163}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>grassland_type</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Natural Grassland  SOC content for 2030 - Only Cattle - Average developing world cattle productivity</t>
   </si>
   <si>
-    <t>LEAFs_dir() / SOC/rasters"</t>
-  </si>
-  <si>
     <t>cattle_hps</t>
   </si>
   <si>
@@ -91,37 +88,31 @@
     <t>Natural Grassland  SOC content for 2030 - All Animals, including  Cattle - Low developing world cattle productivity</t>
   </si>
   <si>
-    <t>_resolve_data_path("soil_weather",  "uhth_pet_locationonly.tif")</t>
-  </si>
-  <si>
-    <t>[_resolve_data_path("grasslands",  "livestock",  "grassland_cattle_other_avgdwprod_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>_resolve_data_path(soil_weather",  "uhth_pet_locationonly.tif")"</t>
-  </si>
-  <si>
-    <t>[_resolve_data_path(grasslands",  "livestock",  "grassland_cattle_other_hpsdwprod_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>[_resolve_data_path(grasslands",  "livestock",  "grassland_cattle_other_lpsdwprod_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>[ _resolve_data_path(grasslands",  "livestock",  "grassland_sheep_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>[ _resolve_data_path(grasslands",  "livestock",  "grassland_goat_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>[ _resolve_data_path(grasslands",  "livestock",  "grassland_sheep_annual_fym.tif"), _resolve_data_path("grasslands",  "livestock",  "grassland_goat_annual_fym.tif"),     _resolve_data_path("grasslands",  "livestock",  "grassland_cattle_other_avgdwprod_annual_fym.tif")]</t>
-  </si>
-  <si>
-    <t>data_path("land_use",  "lu_Grassland.tif")</t>
-  </si>
-  <si>
-    <t>data_path(land_use",  "lu_Grassland.tif")"</t>
-  </si>
-  <si>
-    <t>data_path(land_use",  "lu_Grassland.tif")</t>
+    <t>../data/land_use/lu_Grassland.tif</t>
+  </si>
+  <si>
+    <t>../data/soil_weather/uhth_pet_locationonly.tif</t>
+  </si>
+  <si>
+    <t>../LEAFs/SOC/rasters</t>
+  </si>
+  <si>
+    <t>["../data/grasslands/livestock/grassland_cattle_other_avgdw_annual_fym.tif"]</t>
+  </si>
+  <si>
+    <t>["../data/grasslands/livestock/grassland_cattle_other_hpsdw_annual_fym.tif"]</t>
+  </si>
+  <si>
+    <t>["../data/grasslands/livestock/grassland_cattle_other_lpsdw_annual_fym.tif"]</t>
+  </si>
+  <si>
+    <t>["../data/grasslands/livestock/grassland_sheep_annual_fym.tif"]</t>
+  </si>
+  <si>
+    <t>["../data/grasslands/livestock/grassland_goat_annual_fym.tif"]</t>
+  </si>
+  <si>
+    <t>[ "../data/grasslands/livestock/grassland_sheep_annual_fym.tif", "../data/grasslands/livestock/grassland_goat_annual_fym.tif", "../data/grasslands/livestock/grassland_cattle_other_avgdw_annual_fym.tif"]</t>
   </si>
 </sst>
 </file>
@@ -985,7 +976,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1029,10 +1020,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -1041,13 +1032,13 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -1058,25 +1049,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>100</v>
@@ -1087,25 +1078,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <v>100</v>
@@ -1116,25 +1107,25 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>100</v>
@@ -1145,25 +1136,25 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I6">
         <v>100</v>
@@ -1174,25 +1165,25 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I7">
         <v>100</v>

</xml_diff>